<commit_message>
feat: further data exploration / missing & unknown
</commit_message>
<xml_diff>
--- a/DIAS Information Levels - Attributes 2017.xlsx
+++ b/DIAS Information Levels - Attributes 2017.xlsx
@@ -6261,4 +6261,10 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/internal/2005/internalDocumentation"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=docMetadata/LabelInfo.xml><?xml version="1.0" encoding="utf-8"?>
+<clbl:labelList xmlns:clbl="http://schemas.microsoft.com/office/2020/mipLabelMetadata">
+  <clbl:label id="{42f063bf-ce3a-473c-8609-3866002c85b0}" enabled="1" method="Standard" siteId="{b914a242-e718-443b-a47c-6b4c649d8c0a}" contentBits="0" removed="0"/>
+</clbl:labelList>
 </file>
</xml_diff>